<commit_message>
shard balance update and ch4 map
Fixing bonus orbs from early levels
Increasing shard cost for units and upgrades after each upgrade
</commit_message>
<xml_diff>
--- a/Gates of Mansole/DifficultyCurve.xlsx
+++ b/Gates of Mansole/DifficultyCurve.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="11364" windowHeight="3048" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="11370" windowHeight="3045" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Difficulty Curve" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="Chapter2" sheetId="3" r:id="rId3"/>
     <sheet name="Chapter3" sheetId="4" r:id="rId4"/>
     <sheet name="Chapter4" sheetId="5" r:id="rId5"/>
+    <sheet name="UnitCounts" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -23,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="AB4" authorId="0">
+    <comment ref="AB4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -36,7 +37,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CJ4" authorId="0">
+    <comment ref="CJ4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0">
+    <comment ref="O5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0">
+    <comment ref="P5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BG5" authorId="0">
+    <comment ref="BG5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BT5" authorId="0">
+    <comment ref="BT5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DW5" authorId="0">
+    <comment ref="DW5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FN5" authorId="0">
+    <comment ref="FN5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CB6" authorId="0">
+    <comment ref="CB6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3192" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3218" uniqueCount="424">
   <si>
     <t>Level</t>
   </si>
@@ -1376,6 +1377,75 @@
   </si>
   <si>
     <t>TTOSSE</t>
+  </si>
+  <si>
+    <t>Chapter 1</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Chapter 2</t>
+  </si>
+  <si>
+    <t>Chapter 3</t>
+  </si>
+  <si>
+    <t>Chapter 4</t>
+  </si>
+  <si>
+    <t>Shards Gained</t>
+  </si>
+  <si>
+    <t>Orbs Gained</t>
+  </si>
+  <si>
+    <t>Bonus Orbs</t>
+  </si>
+  <si>
+    <t>Expected Purchase</t>
+  </si>
+  <si>
+    <t>Upgrade Shepherd</t>
+  </si>
+  <si>
+    <t>Unlock Evangelist</t>
+  </si>
+  <si>
+    <t>Start with Shepherd</t>
+  </si>
+  <si>
+    <t>Unlock Shield</t>
+  </si>
+  <si>
+    <t>Unlock Elders</t>
+  </si>
+  <si>
+    <t>Unlock Orators</t>
+  </si>
+  <si>
+    <t>Unlock Teacher</t>
+  </si>
+  <si>
+    <t>Upgrade Evangelist</t>
+  </si>
+  <si>
+    <t>Upgrade Teacher</t>
+  </si>
+  <si>
+    <t>Upgrade Elder</t>
+  </si>
+  <si>
+    <t>Upgrade Orator</t>
+  </si>
+  <si>
+    <t>Unlock Ballista</t>
+  </si>
+  <si>
+    <t>Unlock Earthquake</t>
+  </si>
+  <si>
+    <t>Unlock Catapult</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1489,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1462,11 +1532,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1481,6 +1569,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1490,6 +1581,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1815,13 +1909,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="181380224"/>
-        <c:axId val="181381760"/>
+        <c:axId val="285637320"/>
+        <c:axId val="285633792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181380224"/>
+        <c:axId val="285637320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,7 +1923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181381760"/>
+        <c:crossAx val="285633792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1838,7 +1931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181381760"/>
+        <c:axId val="285633792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,7 +1942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181380224"/>
+        <c:crossAx val="285637320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1948,7 +2041,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1983,7 +2076,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2198,12 +2291,12 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2220,7 +2313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2243,7 +2336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2269,7 +2362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2295,7 +2388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2321,7 +2414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2347,7 +2440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2373,7 +2466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2390,7 +2483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2407,7 +2500,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2424,7 +2517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2441,7 +2534,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2461,7 +2554,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2487,7 +2580,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2513,7 +2606,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2539,7 +2632,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2565,7 +2658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
         <v>37</v>
       </c>
@@ -2576,7 +2669,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
         <v>38</v>
       </c>
@@ -2587,7 +2680,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
         <v>43</v>
       </c>
@@ -2598,7 +2691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
         <v>108</v>
       </c>
@@ -2609,27 +2702,27 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H25" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:12" x14ac:dyDescent="0.25">
       <c r="I28" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>38</v>
       </c>
@@ -2640,7 +2733,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>43</v>
       </c>
@@ -2651,7 +2744,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>105</v>
       </c>
@@ -2662,7 +2755,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>108</v>
       </c>
@@ -2673,7 +2766,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
         <v>109</v>
       </c>
@@ -2695,76 +2788,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GI16"/>
   <sheetViews>
-    <sheetView topLeftCell="FR1" workbookViewId="0">
-      <selection activeCell="EQ12" sqref="EQ12"/>
+    <sheetView topLeftCell="BM1" workbookViewId="0">
+      <selection activeCell="BU28" sqref="BU28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="57" max="59" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="93" max="94" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="111" max="115" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="117" max="119" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="136" max="137" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="138" max="139" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="142" max="145" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="161" max="162" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="163" max="164" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="167" max="170" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="177" max="179" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="180" max="181" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="6.6640625" customWidth="1"/>
-    <col min="187" max="187" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="59" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="115" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="117" max="119" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="136" max="137" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="138" max="139" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="142" max="145" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="161" max="162" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="163" max="164" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="167" max="170" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="177" max="179" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="180" max="181" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="6.7109375" customWidth="1"/>
+    <col min="187" max="187" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:191" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2901,7 +2995,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:191" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -3305,7 +3399,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:191" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
@@ -3442,7 +3536,7 @@
         <v>100</v>
       </c>
       <c r="BT3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BU3" t="s">
         <v>17</v>
@@ -3469,7 +3563,7 @@
         <v>6</v>
       </c>
       <c r="CJ3" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="CK3" s="2" t="s">
         <v>53</v>
@@ -3505,7 +3599,7 @@
         <v>100</v>
       </c>
       <c r="CY3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="CZ3" t="s">
         <v>19</v>
@@ -3700,7 +3794,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:191" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
@@ -3838,7 +3932,7 @@
         <v>2</v>
       </c>
       <c r="BT4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BU4" t="s">
         <v>17</v>
@@ -3862,7 +3956,7 @@
         <v>2</v>
       </c>
       <c r="CJ4" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="CK4" s="2" t="s">
         <v>52</v>
@@ -3895,7 +3989,7 @@
         <v>3</v>
       </c>
       <c r="CY4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="CZ4" t="s">
         <v>19</v>
@@ -4084,7 +4178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:191" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
@@ -4228,7 +4322,7 @@
         <v>2</v>
       </c>
       <c r="BT5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BU5" t="s">
         <v>17</v>
@@ -4285,7 +4379,7 @@
         <v>1</v>
       </c>
       <c r="CY5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="CZ5" t="s">
         <v>19</v>
@@ -4474,7 +4568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:191" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>18</v>
@@ -4612,7 +4706,7 @@
         <v>0</v>
       </c>
       <c r="BT6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BU6" t="s">
         <v>17</v>
@@ -4669,7 +4763,7 @@
         <v>0</v>
       </c>
       <c r="CY6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="CZ6" t="s">
         <v>19</v>
@@ -4858,7 +4952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:191" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -4960,7 +5054,7 @@
         <v>17</v>
       </c>
       <c r="CJ7" s="2" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="CK7" s="2" t="s">
         <v>115</v>
@@ -4993,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="CY7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="CZ7" t="s">
         <v>19</v>
@@ -5164,7 +5258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:191" x14ac:dyDescent="0.25">
       <c r="J8" s="6" t="s">
         <v>43</v>
       </c>
@@ -5211,7 +5305,7 @@
         <v>17</v>
       </c>
       <c r="CJ8" s="2" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="CK8" s="2" t="s">
         <v>113</v>
@@ -5244,7 +5338,7 @@
         <v>6</v>
       </c>
       <c r="CY8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="CZ8" t="s">
         <v>19</v>
@@ -5376,7 +5470,79 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:191" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>18</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <v>8</v>
+      </c>
+      <c r="U9">
+        <v>8</v>
+      </c>
+      <c r="V9">
+        <v>39</v>
+      </c>
+      <c r="AB9">
+        <v>3</v>
+      </c>
+      <c r="AC9">
+        <v>3</v>
+      </c>
+      <c r="AD9">
+        <v>3</v>
+      </c>
+      <c r="AE9">
+        <v>5</v>
+      </c>
+      <c r="AF9">
+        <v>8</v>
+      </c>
+      <c r="AG9">
+        <v>10</v>
+      </c>
+      <c r="AH9">
+        <v>10</v>
+      </c>
+      <c r="AI9">
+        <v>12</v>
+      </c>
+      <c r="AJ9">
+        <v>54</v>
+      </c>
       <c r="AS9" s="5"/>
       <c r="BZ9" t="s">
         <v>63</v>
@@ -5439,7 +5605,73 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:191" x14ac:dyDescent="0.25">
+      <c r="AP10">
+        <v>4</v>
+      </c>
+      <c r="AQ10">
+        <v>5</v>
+      </c>
+      <c r="AR10">
+        <v>5</v>
+      </c>
+      <c r="AS10">
+        <v>8</v>
+      </c>
+      <c r="AT10">
+        <v>11</v>
+      </c>
+      <c r="AU10">
+        <v>10</v>
+      </c>
+      <c r="AV10">
+        <v>15</v>
+      </c>
+      <c r="AW10">
+        <v>15</v>
+      </c>
+      <c r="AX10">
+        <v>73</v>
+      </c>
+      <c r="BD10">
+        <v>4</v>
+      </c>
+      <c r="BE10">
+        <v>8</v>
+      </c>
+      <c r="BF10">
+        <v>8</v>
+      </c>
+      <c r="BG10">
+        <v>8</v>
+      </c>
+      <c r="BH10">
+        <v>10</v>
+      </c>
+      <c r="BI10">
+        <v>12</v>
+      </c>
+      <c r="BJ10">
+        <v>10</v>
+      </c>
+      <c r="BK10">
+        <v>14</v>
+      </c>
+      <c r="BL10">
+        <v>14</v>
+      </c>
+      <c r="BM10">
+        <v>20</v>
+      </c>
+      <c r="BN10">
+        <v>108</v>
+      </c>
+      <c r="BV10">
+        <v>8</v>
+      </c>
+      <c r="CD10">
+        <v>12</v>
+      </c>
       <c r="CM10" s="5"/>
       <c r="EF10" s="5"/>
       <c r="FI10" s="5"/>
@@ -5451,8 +5683,112 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:191" x14ac:dyDescent="0.3">
-      <c r="EF11" s="5"/>
+    <row r="11" spans="1:191" x14ac:dyDescent="0.25">
+      <c r="CJ11">
+        <v>8</v>
+      </c>
+      <c r="CK11">
+        <v>9</v>
+      </c>
+      <c r="CL11">
+        <v>14</v>
+      </c>
+      <c r="CM11">
+        <v>12</v>
+      </c>
+      <c r="CN11">
+        <v>12</v>
+      </c>
+      <c r="CO11">
+        <v>16</v>
+      </c>
+      <c r="CP11">
+        <v>18</v>
+      </c>
+      <c r="CQ11">
+        <v>15</v>
+      </c>
+      <c r="CR11">
+        <v>24</v>
+      </c>
+      <c r="CS11">
+        <v>128</v>
+      </c>
+      <c r="DA11">
+        <v>12</v>
+      </c>
+      <c r="DG11">
+        <v>5</v>
+      </c>
+      <c r="DH11">
+        <v>5</v>
+      </c>
+      <c r="DI11">
+        <v>5</v>
+      </c>
+      <c r="DJ11">
+        <v>5</v>
+      </c>
+      <c r="DK11">
+        <v>8</v>
+      </c>
+      <c r="DL11">
+        <v>10</v>
+      </c>
+      <c r="DM11">
+        <v>10</v>
+      </c>
+      <c r="DN11">
+        <v>10</v>
+      </c>
+      <c r="DO11">
+        <v>13</v>
+      </c>
+      <c r="DP11">
+        <v>15</v>
+      </c>
+      <c r="DQ11">
+        <v>86</v>
+      </c>
+      <c r="DZ11">
+        <v>15</v>
+      </c>
+      <c r="EF11" s="5">
+        <v>5</v>
+      </c>
+      <c r="EG11">
+        <v>5</v>
+      </c>
+      <c r="EH11">
+        <v>10</v>
+      </c>
+      <c r="EI11">
+        <v>10</v>
+      </c>
+      <c r="EJ11">
+        <v>10</v>
+      </c>
+      <c r="EK11">
+        <v>13</v>
+      </c>
+      <c r="EL11">
+        <v>10</v>
+      </c>
+      <c r="EM11">
+        <v>10</v>
+      </c>
+      <c r="EN11">
+        <v>15</v>
+      </c>
+      <c r="EO11">
+        <v>17</v>
+      </c>
+      <c r="EP11">
+        <v>105</v>
+      </c>
+      <c r="EY11">
+        <v>18</v>
+      </c>
       <c r="FD11" s="8"/>
       <c r="FE11" s="9"/>
       <c r="FF11" s="9"/>
@@ -5470,7 +5806,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:191" x14ac:dyDescent="0.25">
       <c r="FD12" s="8"/>
       <c r="FE12" s="9"/>
       <c r="FF12" s="9"/>
@@ -5494,31 +5830,84 @@
       <c r="GH12" s="9"/>
       <c r="GI12" s="9"/>
     </row>
-    <row r="13" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:191" x14ac:dyDescent="0.25">
       <c r="FD13" s="8"/>
-      <c r="FE13" s="9"/>
-      <c r="FF13" s="9"/>
-      <c r="FG13" s="9"/>
-      <c r="FH13" s="9"/>
-      <c r="FI13" s="9"/>
-      <c r="FJ13" s="9"/>
-      <c r="FK13" s="9"/>
-      <c r="FL13" s="9"/>
-      <c r="FM13" s="9"/>
-      <c r="FN13" s="9"/>
-      <c r="FY13" s="9"/>
-      <c r="FZ13" s="9"/>
-      <c r="GA13" s="9"/>
-      <c r="GB13" s="9"/>
-      <c r="GC13" s="9"/>
-      <c r="GD13" s="9"/>
-      <c r="GE13" s="9"/>
-      <c r="GF13" s="9"/>
-      <c r="GG13" s="9"/>
+      <c r="FE13" s="9">
+        <v>6</v>
+      </c>
+      <c r="FF13" s="9">
+        <v>6</v>
+      </c>
+      <c r="FG13" s="9">
+        <v>12</v>
+      </c>
+      <c r="FH13" s="9">
+        <v>12</v>
+      </c>
+      <c r="FI13" s="9">
+        <v>16</v>
+      </c>
+      <c r="FJ13" s="9">
+        <v>12</v>
+      </c>
+      <c r="FK13" s="9">
+        <v>12</v>
+      </c>
+      <c r="FL13" s="9">
+        <v>18</v>
+      </c>
+      <c r="FM13" s="9">
+        <v>20</v>
+      </c>
+      <c r="FN13" s="9">
+        <v>10</v>
+      </c>
+      <c r="FO13" s="5">
+        <v>136</v>
+      </c>
+      <c r="FU13">
+        <v>12</v>
+      </c>
+      <c r="FV13">
+        <v>12</v>
+      </c>
+      <c r="FW13">
+        <v>16</v>
+      </c>
+      <c r="FX13">
+        <v>12</v>
+      </c>
+      <c r="FY13" s="9">
+        <v>12</v>
+      </c>
+      <c r="FZ13" s="9">
+        <v>12</v>
+      </c>
+      <c r="GA13" s="9">
+        <v>18</v>
+      </c>
+      <c r="GB13" s="9">
+        <v>12</v>
+      </c>
+      <c r="GC13" s="9">
+        <v>18</v>
+      </c>
+      <c r="GD13" s="9">
+        <v>24</v>
+      </c>
+      <c r="GE13" s="9">
+        <v>18</v>
+      </c>
+      <c r="GF13" s="9">
+        <v>15</v>
+      </c>
+      <c r="GG13" s="9">
+        <v>181</v>
+      </c>
       <c r="GH13" s="9"/>
       <c r="GI13" s="9"/>
     </row>
-    <row r="14" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:191" x14ac:dyDescent="0.25">
       <c r="FD14" s="8"/>
       <c r="FE14" s="9"/>
       <c r="FF14" s="9"/>
@@ -5542,7 +5931,7 @@
       <c r="GH14" s="9"/>
       <c r="GI14" s="9"/>
     </row>
-    <row r="15" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:191" x14ac:dyDescent="0.25">
       <c r="FD15" s="8"/>
       <c r="FE15" s="9"/>
       <c r="FF15" s="9"/>
@@ -5555,7 +5944,7 @@
       <c r="FM15" s="9"/>
       <c r="FN15" s="9"/>
     </row>
-    <row r="16" spans="1:191" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:191" x14ac:dyDescent="0.25">
       <c r="FD16" s="8"/>
       <c r="FE16" s="8"/>
       <c r="FF16" s="8"/>
@@ -5579,66 +5968,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GC9"/>
   <sheetViews>
-    <sheetView topLeftCell="FL1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="64" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="99" max="100" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="131" max="132" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="171" max="172" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="173" max="174" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="175" max="179" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="62" max="64" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="99" max="100" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="131" max="132" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="171" max="172" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="173" max="174" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="175" max="179" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -5775,7 +6164,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:185" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -6116,7 +6505,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:185" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>139</v>
       </c>
@@ -6508,7 +6897,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:185" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6876,7 +7265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:185" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
@@ -7244,7 +7633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:185" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>139</v>
       </c>
@@ -7612,7 +8001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -7915,7 +8304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:185" x14ac:dyDescent="0.25">
       <c r="M8" s="6" t="s">
         <v>43</v>
       </c>
@@ -8196,7 +8585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:185" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:185" x14ac:dyDescent="0.25">
       <c r="AH9" t="s">
         <v>63</v>
       </c>
@@ -8307,112 +8696,111 @@
       <selection activeCell="GV28" sqref="GV28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" customWidth="1"/>
-    <col min="14" max="14" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.6640625" customWidth="1"/>
-    <col min="19" max="19" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.7109375" customWidth="1"/>
+    <col min="19" max="19" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="63" width="12" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="73" max="74" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="75" max="79" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="89" max="91" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="93" max="94" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="104" max="105" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="107" max="108" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="110" max="112" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="119" max="120" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="121" max="122" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="124" max="125" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="126" max="127" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="147" max="148" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="150" max="151" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="152" max="153" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="79" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="89" max="91" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="104" max="105" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="107" max="108" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="110" max="112" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="119" max="120" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="121" max="122" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="124" max="125" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="126" max="127" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="147" max="148" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="150" max="151" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="152" max="153" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="165" max="165" width="2" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="173" max="174" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="176" max="176" width="2" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="195" max="196" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="197" max="198" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="199" max="200" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="195" max="196" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="197" max="198" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="199" max="200" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="202" max="202" width="10" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="207" max="207" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:210" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -8549,7 +8937,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:210" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -8989,7 +9377,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:210" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -9489,7 +9877,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:210" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -9971,7 +10359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:210" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -10453,7 +10841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:210" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -10935,7 +11323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:210" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -11310,7 +11698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:210" x14ac:dyDescent="0.25">
       <c r="N8" s="6" t="s">
         <v>43</v>
       </c>
@@ -11544,7 +11932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:210" x14ac:dyDescent="0.25">
       <c r="AP9" t="s">
         <v>63</v>
       </c>
@@ -11626,7 +12014,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:210" x14ac:dyDescent="0.25">
       <c r="GL10">
         <v>7</v>
       </c>
@@ -11670,7 +12058,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:210" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:210" x14ac:dyDescent="0.25">
       <c r="GK11" t="s">
         <v>63</v>
       </c>
@@ -11707,120 +12095,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="AY1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="GM10" sqref="GM10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="32" width="10" bestFit="1" customWidth="1"/>
     <col min="33" max="34" width="10" customWidth="1"/>
-    <col min="35" max="35" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="41" max="42" width="10" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="10" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="55" max="56" width="10" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="60" max="62" width="10" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="72" max="73" width="10" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="77" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="80" max="81" width="10" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="87" max="89" width="10" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="101" max="102" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="101" max="102" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="10" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="107" max="108" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="107" max="108" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="109" max="110" width="10" bestFit="1" customWidth="1"/>
-    <col min="111" max="112" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="112" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="113" max="116" width="10" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="118" max="119" width="10" bestFit="1" customWidth="1"/>
-    <col min="120" max="121" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="121" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="122" max="123" width="10" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="131" max="132" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="131" max="132" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="135" max="137" width="10" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="139" max="140" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="141" max="142" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="139" max="140" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="141" max="142" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="143" max="143" width="10" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="154" max="155" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="152" max="153" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="154" max="155" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="156" max="156" width="2" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="161" max="162" width="10" bestFit="1" customWidth="1"/>
-    <col min="163" max="166" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="163" max="166" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="167" max="168" width="10" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="170" max="172" width="10" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="176" max="176" width="6" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="182" max="183" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="181" max="183" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="185" max="186" width="2" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="189" max="189" width="6" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="194" max="194" width="10" bestFit="1" customWidth="1"/>
-    <col min="195" max="196" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="203" max="204" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="206" max="207" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="195" max="196" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="203" max="204" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="206" max="207" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="209" max="209" width="6" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="7.44140625" customWidth="1"/>
-    <col min="211" max="211" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="7.42578125" customWidth="1"/>
+    <col min="211" max="211" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:209" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -11957,7 +12343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:209" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -12364,7 +12750,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:209" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -12861,7 +13247,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:209" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -13349,7 +13735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:209" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -13837,7 +14223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:209" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -14325,7 +14711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:209" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -14713,7 +15099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:209" x14ac:dyDescent="0.25">
       <c r="O8" s="6" t="s">
         <v>43</v>
       </c>
@@ -15009,7 +15395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:209" x14ac:dyDescent="0.25">
       <c r="AW9" t="s">
         <v>63</v>
       </c>
@@ -15198,7 +15584,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:209" x14ac:dyDescent="0.25">
       <c r="DR10" t="s">
         <v>63</v>
       </c>
@@ -15258,7 +15644,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="11" spans="1:209" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:209" x14ac:dyDescent="0.25">
       <c r="GI11" t="s">
         <v>63</v>
       </c>
@@ -15296,4 +15682,2732 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1" s="12">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12">
+        <v>5</v>
+      </c>
+      <c r="I1" s="12">
+        <v>6</v>
+      </c>
+      <c r="J1" s="12">
+        <v>7</v>
+      </c>
+      <c r="K1" s="12">
+        <v>8</v>
+      </c>
+      <c r="L1" s="12">
+        <v>9</v>
+      </c>
+      <c r="M1" s="12">
+        <v>10</v>
+      </c>
+      <c r="N1" s="12">
+        <v>11</v>
+      </c>
+      <c r="O1" s="12">
+        <v>12</v>
+      </c>
+      <c r="P1" s="12">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="12">
+        <v>14</v>
+      </c>
+      <c r="R1" s="12">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>SUM(D3:R3)</f>
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="T3">
+        <f>C3 * 2</f>
+        <v>36</v>
+      </c>
+      <c r="U3">
+        <v>8</v>
+      </c>
+      <c r="W3">
+        <f>_xlfn.CEILING.MATH(T3 * 0.05) + U3</f>
+        <v>10</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C17" si="0">SUM(D4:R4)</f>
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T65" si="1">C4 * 2</f>
+        <v>78</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4" si="2">_xlfn.CEILING.MATH(T4 * 0.05) + U4</f>
+        <v>7</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>12</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <f>_xlfn.CEILING.MATH(T5 * 0.05) + U5</f>
+        <v>10</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <f>_xlfn.CEILING.MATH(T6 * 0.05) + U6</f>
+        <v>13</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>14</v>
+      </c>
+      <c r="L7">
+        <v>14</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="W7">
+        <f>_xlfn.CEILING.MATH(T7 * 0.05) + U7</f>
+        <v>17</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="U8">
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <f>(T8*0.5) + U8</f>
+        <v>13</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="W9">
+        <f>(T9*0.5) + U9</f>
+        <v>17</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>18</v>
+      </c>
+      <c r="K10">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>24</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="U10">
+        <v>6</v>
+      </c>
+      <c r="W10">
+        <f>_xlfn.CEILING.MATH(T10 * 0.05) + U10</f>
+        <v>19</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="U11">
+        <v>6</v>
+      </c>
+      <c r="W11">
+        <f>(T11*0.5) + U11</f>
+        <v>18</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>13</v>
+      </c>
+      <c r="M12">
+        <v>15</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>172</v>
+      </c>
+      <c r="U12">
+        <v>7</v>
+      </c>
+      <c r="W12">
+        <f>_xlfn.CEILING.MATH(T12 * 0.05) + U12</f>
+        <v>16</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="U13">
+        <v>6</v>
+      </c>
+      <c r="W13">
+        <f>(T13*0.5) + U13</f>
+        <v>21</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>15</v>
+      </c>
+      <c r="M14">
+        <v>17</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="U14">
+        <v>6</v>
+      </c>
+      <c r="W14">
+        <f>_xlfn.CEILING.MATH(T14 * 0.05) + U14</f>
+        <v>17</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="U15">
+        <v>7</v>
+      </c>
+      <c r="W15">
+        <f>(T15*0.5) + U15</f>
+        <v>25</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="D16" s="9">
+        <v>6</v>
+      </c>
+      <c r="E16" s="9">
+        <v>6</v>
+      </c>
+      <c r="F16" s="9">
+        <v>12</v>
+      </c>
+      <c r="G16" s="9">
+        <v>12</v>
+      </c>
+      <c r="H16" s="9">
+        <v>16</v>
+      </c>
+      <c r="I16" s="9">
+        <v>12</v>
+      </c>
+      <c r="J16" s="9">
+        <v>12</v>
+      </c>
+      <c r="K16" s="9">
+        <v>18</v>
+      </c>
+      <c r="L16" s="9">
+        <v>20</v>
+      </c>
+      <c r="M16" s="9">
+        <v>10</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>248</v>
+      </c>
+      <c r="U16">
+        <v>7</v>
+      </c>
+      <c r="W16">
+        <f>_xlfn.CEILING.MATH(T16 * 0.05) + U16</f>
+        <v>20</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17" s="9">
+        <v>12</v>
+      </c>
+      <c r="I17" s="9">
+        <v>12</v>
+      </c>
+      <c r="J17" s="9">
+        <v>18</v>
+      </c>
+      <c r="K17" s="9">
+        <v>12</v>
+      </c>
+      <c r="L17" s="9">
+        <v>18</v>
+      </c>
+      <c r="M17" s="9">
+        <v>24</v>
+      </c>
+      <c r="N17" s="9">
+        <v>18</v>
+      </c>
+      <c r="O17" s="9">
+        <v>15</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>362</v>
+      </c>
+      <c r="U17">
+        <v>8</v>
+      </c>
+      <c r="W17">
+        <f>_xlfn.CEILING.MATH(T17 * 0.05) + U17</f>
+        <v>27</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f>SUM(D19:R19)</f>
+        <v>56</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>10</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="U19">
+        <v>7</v>
+      </c>
+      <c r="W19">
+        <f>_xlfn.CEILING.MATH(T19 * 0.05) + U19</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="13">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:C33" si="3">SUM(D20:R20)</f>
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="U20">
+        <v>8</v>
+      </c>
+      <c r="W20">
+        <f>(T20*0.5) + U20</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="13">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="U21">
+        <v>9</v>
+      </c>
+      <c r="W21">
+        <f>(T21*0.5) + U21</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="13">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="U22">
+        <v>10</v>
+      </c>
+      <c r="W22">
+        <f>(T22*0.5) + U22</f>
+        <v>28</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="13">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>155</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>15</v>
+      </c>
+      <c r="M23">
+        <v>20</v>
+      </c>
+      <c r="N23">
+        <v>15</v>
+      </c>
+      <c r="O23">
+        <v>15</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>310</v>
+      </c>
+      <c r="U23">
+        <v>11</v>
+      </c>
+      <c r="W23">
+        <f>_xlfn.CEILING.MATH(T23 * 0.05) + U23</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="13">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>130</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>16</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>12</v>
+      </c>
+      <c r="I24">
+        <v>12</v>
+      </c>
+      <c r="J24">
+        <v>18</v>
+      </c>
+      <c r="K24">
+        <v>12</v>
+      </c>
+      <c r="L24">
+        <v>24</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="U24">
+        <v>10</v>
+      </c>
+      <c r="W24">
+        <f>_xlfn.CEILING.MATH(T24 * 0.05) + U24</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="13">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>148</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>18</v>
+      </c>
+      <c r="F25">
+        <v>16</v>
+      </c>
+      <c r="G25">
+        <v>12</v>
+      </c>
+      <c r="H25">
+        <v>18</v>
+      </c>
+      <c r="I25">
+        <v>12</v>
+      </c>
+      <c r="J25">
+        <v>18</v>
+      </c>
+      <c r="K25">
+        <v>24</v>
+      </c>
+      <c r="L25">
+        <v>18</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>296</v>
+      </c>
+      <c r="U25">
+        <v>10</v>
+      </c>
+      <c r="W25">
+        <f>_xlfn.CEILING.MATH(T25 * 0.05) + U25</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="13">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>18</v>
+      </c>
+      <c r="G26">
+        <v>18</v>
+      </c>
+      <c r="H26">
+        <v>12</v>
+      </c>
+      <c r="I26">
+        <v>18</v>
+      </c>
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="K26">
+        <v>24</v>
+      </c>
+      <c r="L26">
+        <v>24</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="U26">
+        <v>11</v>
+      </c>
+      <c r="W26">
+        <f>_xlfn.CEILING.MATH(T26 * 0.05) + U26</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="13">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="U27">
+        <v>11</v>
+      </c>
+      <c r="W27">
+        <f>(T27*0.5) + U27</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="13">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="D28">
+        <v>18</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="U28">
+        <v>12</v>
+      </c>
+      <c r="W28">
+        <f>(T28*0.5) + U28</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="13">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>186</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>18</v>
+      </c>
+      <c r="G29">
+        <v>18</v>
+      </c>
+      <c r="H29">
+        <v>18</v>
+      </c>
+      <c r="I29">
+        <v>18</v>
+      </c>
+      <c r="J29">
+        <v>18</v>
+      </c>
+      <c r="K29">
+        <v>24</v>
+      </c>
+      <c r="L29">
+        <v>24</v>
+      </c>
+      <c r="M29">
+        <v>24</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="1"/>
+        <v>372</v>
+      </c>
+      <c r="U29">
+        <v>11</v>
+      </c>
+      <c r="W29">
+        <f>_xlfn.CEILING.MATH(T29 * 0.05) + U29</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="13">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="D30">
+        <v>19</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="U30">
+        <v>11</v>
+      </c>
+      <c r="W30">
+        <f>(T30*0.5) + U30</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="13">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="D31">
+        <v>19</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="U31">
+        <v>12</v>
+      </c>
+      <c r="W31">
+        <f>(T31*0.5) + U31</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="13">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="U32">
+        <v>12</v>
+      </c>
+      <c r="W32">
+        <f>(T32*0.5) + U32</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="13">
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="3"/>
+        <v>245</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>18</v>
+      </c>
+      <c r="G33">
+        <v>18</v>
+      </c>
+      <c r="H33">
+        <v>18</v>
+      </c>
+      <c r="I33">
+        <v>18</v>
+      </c>
+      <c r="J33">
+        <v>18</v>
+      </c>
+      <c r="K33">
+        <v>18</v>
+      </c>
+      <c r="L33">
+        <v>24</v>
+      </c>
+      <c r="M33">
+        <v>26</v>
+      </c>
+      <c r="N33">
+        <v>18</v>
+      </c>
+      <c r="O33">
+        <v>24</v>
+      </c>
+      <c r="P33">
+        <v>21</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>490</v>
+      </c>
+      <c r="U33">
+        <v>13</v>
+      </c>
+      <c r="W33">
+        <f>_xlfn.CEILING.MATH(T33 * 0.05) + U33</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35" s="13">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <f>SUM(D35:R35)</f>
+        <v>126</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <v>12</v>
+      </c>
+      <c r="I35">
+        <v>12</v>
+      </c>
+      <c r="J35">
+        <v>16</v>
+      </c>
+      <c r="K35">
+        <v>16</v>
+      </c>
+      <c r="L35">
+        <v>16</v>
+      </c>
+      <c r="M35">
+        <v>14</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+      <c r="U35">
+        <v>11</v>
+      </c>
+      <c r="W35">
+        <f t="shared" ref="W35:W45" si="4">_xlfn.CEILING.MATH(T35 * 0.05) + U35</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" s="13">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:C49" si="5">SUM(D36:R36)</f>
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="U36">
+        <v>11</v>
+      </c>
+      <c r="W36">
+        <f>(T36*0.5) + U36</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37" s="13">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="5"/>
+        <v>127</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>13</v>
+      </c>
+      <c r="G37">
+        <v>13</v>
+      </c>
+      <c r="H37">
+        <v>12</v>
+      </c>
+      <c r="I37">
+        <v>10</v>
+      </c>
+      <c r="J37">
+        <v>15</v>
+      </c>
+      <c r="K37">
+        <v>10</v>
+      </c>
+      <c r="L37">
+        <v>15</v>
+      </c>
+      <c r="M37">
+        <v>19</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="1"/>
+        <v>254</v>
+      </c>
+      <c r="U37">
+        <v>12</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38" s="13">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <v>18</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="U38">
+        <v>12</v>
+      </c>
+      <c r="W38">
+        <f>(T38*0.5) + U38</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39" s="13">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="5"/>
+        <v>204</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>13</v>
+      </c>
+      <c r="G39">
+        <v>12</v>
+      </c>
+      <c r="H39">
+        <v>12</v>
+      </c>
+      <c r="I39">
+        <v>16</v>
+      </c>
+      <c r="J39">
+        <v>16</v>
+      </c>
+      <c r="K39">
+        <v>16</v>
+      </c>
+      <c r="L39">
+        <v>16</v>
+      </c>
+      <c r="M39">
+        <v>20</v>
+      </c>
+      <c r="N39">
+        <v>20</v>
+      </c>
+      <c r="O39">
+        <v>20</v>
+      </c>
+      <c r="P39">
+        <v>21</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="1"/>
+        <v>408</v>
+      </c>
+      <c r="U39">
+        <v>13</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40" s="13">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="5"/>
+        <v>182</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <v>12</v>
+      </c>
+      <c r="F40">
+        <v>18</v>
+      </c>
+      <c r="G40">
+        <v>18</v>
+      </c>
+      <c r="H40">
+        <v>18</v>
+      </c>
+      <c r="I40">
+        <v>18</v>
+      </c>
+      <c r="J40">
+        <v>18</v>
+      </c>
+      <c r="K40">
+        <v>18</v>
+      </c>
+      <c r="L40">
+        <v>24</v>
+      </c>
+      <c r="M40">
+        <v>26</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="1"/>
+        <v>364</v>
+      </c>
+      <c r="U40">
+        <v>12</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41" s="13">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="5"/>
+        <v>183</v>
+      </c>
+      <c r="D41">
+        <v>15</v>
+      </c>
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="F41">
+        <v>18</v>
+      </c>
+      <c r="G41">
+        <v>15</v>
+      </c>
+      <c r="H41">
+        <v>15</v>
+      </c>
+      <c r="I41">
+        <v>20</v>
+      </c>
+      <c r="J41">
+        <v>20</v>
+      </c>
+      <c r="K41">
+        <v>20</v>
+      </c>
+      <c r="L41">
+        <v>20</v>
+      </c>
+      <c r="M41">
+        <v>20</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="1"/>
+        <v>366</v>
+      </c>
+      <c r="U41">
+        <v>12</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" s="13">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="D42">
+        <v>15</v>
+      </c>
+      <c r="E42">
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <v>16</v>
+      </c>
+      <c r="G42">
+        <v>20</v>
+      </c>
+      <c r="H42">
+        <v>20</v>
+      </c>
+      <c r="I42">
+        <v>20</v>
+      </c>
+      <c r="J42">
+        <v>15</v>
+      </c>
+      <c r="K42">
+        <v>20</v>
+      </c>
+      <c r="L42">
+        <v>23</v>
+      </c>
+      <c r="M42">
+        <v>23</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="U42">
+        <v>13</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43" s="13">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="5"/>
+        <v>184</v>
+      </c>
+      <c r="D43">
+        <v>16</v>
+      </c>
+      <c r="E43">
+        <v>16</v>
+      </c>
+      <c r="F43">
+        <v>16</v>
+      </c>
+      <c r="G43">
+        <v>16</v>
+      </c>
+      <c r="H43">
+        <v>16</v>
+      </c>
+      <c r="I43">
+        <v>20</v>
+      </c>
+      <c r="J43">
+        <v>20</v>
+      </c>
+      <c r="K43">
+        <v>20</v>
+      </c>
+      <c r="L43">
+        <v>20</v>
+      </c>
+      <c r="M43">
+        <v>24</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="1"/>
+        <v>368</v>
+      </c>
+      <c r="U43">
+        <v>13</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44" s="13">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="D44">
+        <v>24</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="U44">
+        <v>14</v>
+      </c>
+      <c r="W44">
+        <f>(T44*0.5) + U44</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45" s="13">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="D45">
+        <v>16</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+      <c r="F45">
+        <v>16</v>
+      </c>
+      <c r="G45">
+        <v>16</v>
+      </c>
+      <c r="H45">
+        <v>16</v>
+      </c>
+      <c r="I45">
+        <v>20</v>
+      </c>
+      <c r="J45">
+        <v>20</v>
+      </c>
+      <c r="K45">
+        <v>16</v>
+      </c>
+      <c r="L45">
+        <v>20</v>
+      </c>
+      <c r="M45">
+        <v>24</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="U45">
+        <v>13</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46" s="13">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="D46">
+        <v>17</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="U46">
+        <v>13</v>
+      </c>
+      <c r="W46">
+        <f>(T46*0.5) + U46</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47" s="13">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="D47">
+        <v>20</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="U47">
+        <v>14</v>
+      </c>
+      <c r="W47">
+        <f>(T47*0.5) + U47</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48" s="13">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="D48">
+        <v>22</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="U48">
+        <v>14</v>
+      </c>
+      <c r="W48">
+        <f>(T48*0.5) + U48</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49" s="13">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="5"/>
+        <v>364</v>
+      </c>
+      <c r="D49">
+        <v>16</v>
+      </c>
+      <c r="E49">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>21</v>
+      </c>
+      <c r="G49">
+        <v>21</v>
+      </c>
+      <c r="H49">
+        <v>24</v>
+      </c>
+      <c r="I49">
+        <v>24</v>
+      </c>
+      <c r="J49">
+        <v>21</v>
+      </c>
+      <c r="K49">
+        <v>30</v>
+      </c>
+      <c r="L49">
+        <v>28</v>
+      </c>
+      <c r="M49">
+        <v>34</v>
+      </c>
+      <c r="N49">
+        <v>34</v>
+      </c>
+      <c r="O49">
+        <v>32</v>
+      </c>
+      <c r="P49">
+        <v>42</v>
+      </c>
+      <c r="Q49">
+        <v>21</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="1"/>
+        <v>728</v>
+      </c>
+      <c r="U49">
+        <v>15</v>
+      </c>
+      <c r="W49">
+        <f t="shared" ref="W49:W51" si="6">_xlfn.CEILING.MATH(T49 * 0.05) + U49</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B50" s="14" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>46</v>
+      </c>
+      <c r="B51" s="13">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <f>SUM(D51:R51)</f>
+        <v>204</v>
+      </c>
+      <c r="D51">
+        <v>18</v>
+      </c>
+      <c r="E51">
+        <v>18</v>
+      </c>
+      <c r="F51">
+        <v>16</v>
+      </c>
+      <c r="G51">
+        <v>16</v>
+      </c>
+      <c r="H51">
+        <v>16</v>
+      </c>
+      <c r="I51">
+        <v>20</v>
+      </c>
+      <c r="J51">
+        <v>20</v>
+      </c>
+      <c r="K51">
+        <v>20</v>
+      </c>
+      <c r="L51">
+        <v>18</v>
+      </c>
+      <c r="M51">
+        <v>18</v>
+      </c>
+      <c r="N51">
+        <v>24</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="1"/>
+        <v>408</v>
+      </c>
+      <c r="U51">
+        <v>14</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="B52" s="13">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ref="C52:C65" si="7">SUM(D52:R52)</f>
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>15</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="U52">
+        <v>14</v>
+      </c>
+      <c r="W52">
+        <f>(T52*0.5) + U52</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>48</v>
+      </c>
+      <c r="B53" s="13">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="D53">
+        <v>20</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="U53">
+        <v>15</v>
+      </c>
+      <c r="W53">
+        <f>(T53*0.5) + U53</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>49</v>
+      </c>
+      <c r="B54" s="13">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="D54">
+        <v>20</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="U54">
+        <v>15</v>
+      </c>
+      <c r="W54">
+        <f>(T54*0.5) + U54</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>50</v>
+      </c>
+      <c r="B55" s="13">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="7"/>
+        <v>341</v>
+      </c>
+      <c r="D55">
+        <v>18</v>
+      </c>
+      <c r="E55">
+        <v>18</v>
+      </c>
+      <c r="F55">
+        <v>18</v>
+      </c>
+      <c r="G55">
+        <v>18</v>
+      </c>
+      <c r="H55">
+        <v>28</v>
+      </c>
+      <c r="I55">
+        <v>28</v>
+      </c>
+      <c r="J55">
+        <v>16</v>
+      </c>
+      <c r="K55">
+        <v>24</v>
+      </c>
+      <c r="L55">
+        <v>24</v>
+      </c>
+      <c r="M55">
+        <v>30</v>
+      </c>
+      <c r="N55">
+        <v>30</v>
+      </c>
+      <c r="O55">
+        <v>26</v>
+      </c>
+      <c r="P55">
+        <v>32</v>
+      </c>
+      <c r="Q55">
+        <v>31</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="1"/>
+        <v>682</v>
+      </c>
+      <c r="U55">
+        <v>16</v>
+      </c>
+      <c r="W55">
+        <f t="shared" ref="W55" si="8">_xlfn.CEILING.MATH(T55 * 0.05) + U55</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>51</v>
+      </c>
+      <c r="B56" s="13">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="D56">
+        <v>16</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="U56">
+        <v>15</v>
+      </c>
+      <c r="W56">
+        <f>(T56*0.5) + U56</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>52</v>
+      </c>
+      <c r="B57" s="13">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="7"/>
+        <v>280</v>
+      </c>
+      <c r="D57">
+        <v>28</v>
+      </c>
+      <c r="E57">
+        <v>28</v>
+      </c>
+      <c r="F57">
+        <v>18</v>
+      </c>
+      <c r="G57">
+        <v>18</v>
+      </c>
+      <c r="H57">
+        <v>16</v>
+      </c>
+      <c r="I57">
+        <v>24</v>
+      </c>
+      <c r="J57">
+        <v>30</v>
+      </c>
+      <c r="K57">
+        <v>30</v>
+      </c>
+      <c r="L57">
+        <v>30</v>
+      </c>
+      <c r="M57">
+        <v>26</v>
+      </c>
+      <c r="N57">
+        <v>32</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+      <c r="U57">
+        <v>15</v>
+      </c>
+      <c r="W57">
+        <f t="shared" ref="W57" si="9">_xlfn.CEILING.MATH(T57 * 0.05) + U57</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>53</v>
+      </c>
+      <c r="B58" s="13">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="D58">
+        <v>20</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="U58">
+        <v>16</v>
+      </c>
+      <c r="W58">
+        <f>(T58*0.5) + U58</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>54</v>
+      </c>
+      <c r="B59" s="13">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="D59">
+        <v>18</v>
+      </c>
+      <c r="E59">
+        <v>18</v>
+      </c>
+      <c r="F59">
+        <v>28</v>
+      </c>
+      <c r="G59">
+        <v>28</v>
+      </c>
+      <c r="H59">
+        <v>24</v>
+      </c>
+      <c r="I59">
+        <v>24</v>
+      </c>
+      <c r="J59">
+        <v>34</v>
+      </c>
+      <c r="K59">
+        <v>34</v>
+      </c>
+      <c r="L59">
+        <v>30</v>
+      </c>
+      <c r="M59">
+        <v>30</v>
+      </c>
+      <c r="N59">
+        <v>32</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="U59">
+        <v>16</v>
+      </c>
+      <c r="W59">
+        <f t="shared" ref="W59" si="10">_xlfn.CEILING.MATH(T59 * 0.05) + U59</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>55</v>
+      </c>
+      <c r="B60" s="13">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="D60">
+        <v>28</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="U60">
+        <v>17</v>
+      </c>
+      <c r="W60">
+        <f>(T60*0.5) + U60</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>56</v>
+      </c>
+      <c r="B61" s="13">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+      <c r="D61">
+        <v>18</v>
+      </c>
+      <c r="E61">
+        <v>18</v>
+      </c>
+      <c r="F61">
+        <v>16</v>
+      </c>
+      <c r="G61">
+        <v>16</v>
+      </c>
+      <c r="H61">
+        <v>20</v>
+      </c>
+      <c r="I61">
+        <v>20</v>
+      </c>
+      <c r="J61">
+        <v>20</v>
+      </c>
+      <c r="K61">
+        <v>18</v>
+      </c>
+      <c r="L61">
+        <v>18</v>
+      </c>
+      <c r="M61">
+        <v>16</v>
+      </c>
+      <c r="N61">
+        <v>20</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="U61">
+        <v>16</v>
+      </c>
+      <c r="W61">
+        <f t="shared" ref="W61" si="11">_xlfn.CEILING.MATH(T61 * 0.05) + U61</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>57</v>
+      </c>
+      <c r="B62" s="13">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+      <c r="D62">
+        <v>24</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="U62">
+        <v>17</v>
+      </c>
+      <c r="W62">
+        <f>(T62*0.5) + U62</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>58</v>
+      </c>
+      <c r="B63" s="13">
+        <v>13</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="D63">
+        <v>18</v>
+      </c>
+      <c r="E63">
+        <v>18</v>
+      </c>
+      <c r="F63">
+        <v>22</v>
+      </c>
+      <c r="G63">
+        <v>22</v>
+      </c>
+      <c r="H63">
+        <v>28</v>
+      </c>
+      <c r="I63">
+        <v>28</v>
+      </c>
+      <c r="J63">
+        <v>34</v>
+      </c>
+      <c r="K63">
+        <v>30</v>
+      </c>
+      <c r="L63">
+        <v>30</v>
+      </c>
+      <c r="M63">
+        <v>26</v>
+      </c>
+      <c r="N63">
+        <v>32</v>
+      </c>
+      <c r="T63">
+        <f t="shared" si="1"/>
+        <v>576</v>
+      </c>
+      <c r="U63">
+        <v>18</v>
+      </c>
+      <c r="W63">
+        <f t="shared" ref="W63" si="12">_xlfn.CEILING.MATH(T63 * 0.05) + U63</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>59</v>
+      </c>
+      <c r="B64" s="13">
+        <v>14</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="D64">
+        <v>37</v>
+      </c>
+      <c r="T64">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="U64">
+        <v>19</v>
+      </c>
+      <c r="W64">
+        <f>(T64*0.5) + U64</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>60</v>
+      </c>
+      <c r="B65" s="13">
+        <v>15</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="7"/>
+        <v>516</v>
+      </c>
+      <c r="D65">
+        <v>24</v>
+      </c>
+      <c r="E65">
+        <v>38</v>
+      </c>
+      <c r="F65">
+        <v>36</v>
+      </c>
+      <c r="G65">
+        <v>36</v>
+      </c>
+      <c r="H65">
+        <v>30</v>
+      </c>
+      <c r="I65">
+        <v>21</v>
+      </c>
+      <c r="J65">
+        <v>36</v>
+      </c>
+      <c r="K65">
+        <v>28</v>
+      </c>
+      <c r="L65">
+        <v>36</v>
+      </c>
+      <c r="M65">
+        <v>31</v>
+      </c>
+      <c r="N65">
+        <v>36</v>
+      </c>
+      <c r="O65">
+        <v>36</v>
+      </c>
+      <c r="P65">
+        <v>44</v>
+      </c>
+      <c r="Q65">
+        <v>48</v>
+      </c>
+      <c r="R65">
+        <v>36</v>
+      </c>
+      <c r="T65">
+        <f t="shared" si="1"/>
+        <v>1032</v>
+      </c>
+      <c r="U65">
+        <v>20</v>
+      </c>
+      <c r="W65">
+        <f t="shared" ref="W65" si="13">_xlfn.CEILING.MATH(T65 * 0.05) + U65</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B66" s="13"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B67" s="13"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B68" s="13"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B69" s="13"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B70" s="13"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B71" s="13"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B72" s="13"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B73" s="13"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B74" s="13"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B75" s="13"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B76" s="13"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B77" s="13"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B78" s="13"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B79" s="13"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B80" s="13"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="13"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="13"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="13"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="13"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="13"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="13"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="13"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="13"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="13"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="13"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="13"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>